<commit_message>
REV1 fixes, BOM and Gerber and Drill
</commit_message>
<xml_diff>
--- a/Altium/REV1/Project Outputs for 2024-Badge-Altium-Project-REV1/2024-Badge-BOM-REV1.xlsx
+++ b/Altium/REV1/Project Outputs for 2024-Badge-Altium-Project-REV1/2024-Badge-BOM-REV1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedeaton/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/UNTITLED 2/2024-Badge - REV1.1/Project Outputs for 2024-Badge-Altium-Project-REV1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{13C32A09-B454-A64C-8750-9218E83D5311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4418DAAA-916A-2146-941C-5473F68452F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="11460" windowWidth="35840" windowHeight="10940"/>
   </bookViews>
   <sheets>
     <sheet name="2024-Badge-BOM-REV1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>Designator</t>
   </si>
@@ -199,16 +199,16 @@
     <t>P3</t>
   </si>
   <si>
-    <t>CONN FPC TOP 40POS 0.5MM R/A</t>
+    <t>CONN FPC BOTTOM 40POS 0.5MM R/A</t>
   </si>
   <si>
     <t>Amphenol ICC (FCI)</t>
   </si>
   <si>
-    <t>62684-402100ALF</t>
-  </si>
-  <si>
-    <t>609-1200-1-ND</t>
+    <t>62684-401100AHLF</t>
+  </si>
+  <si>
+    <t>609-62684-401100AHLFTR-ND</t>
   </si>
   <si>
     <t>D3, D4, D5, D6</t>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>1568-1213-ND</t>
+  </si>
+  <si>
+    <t>1568-1213-ND contains 5 each of COM-129865</t>
   </si>
   <si>
     <t>U2</t>
@@ -389,7 +392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -509,8 +512,8 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,8 +539,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,22 +926,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" customWidth="1"/>
-    <col min="7" max="7" width="60.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="84.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -964,7 +967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -986,11 +989,11 @@
       <c r="G2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1012,11 +1015,11 @@
       <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1038,11 +1041,11 @@
       <c r="G4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1064,11 +1067,11 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1090,11 +1093,11 @@
       <c r="G6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1116,11 +1119,11 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -1142,11 +1145,11 @@
       <c r="G8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -1168,11 +1171,11 @@
       <c r="G9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1194,11 +1197,11 @@
       <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -1220,11 +1223,11 @@
       <c r="G11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
@@ -1246,11 +1249,11 @@
       <c r="G12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="10">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
@@ -1272,11 +1275,11 @@
       <c r="G13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
@@ -1296,269 +1299,269 @@
         <v>67</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+        <v>68</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14">
       <c r="A15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="1">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H24" s="1">
+        <v>120</v>
+      </c>
+      <c r="H24" s="10">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to BOM for fab
added a couple comments for the fabricator to know what not to place and the 4-pin header.

this included updating the BOM xls and the ZIP containing the BOM.
</commit_message>
<xml_diff>
--- a/Altium/REV1/Project Outputs for 2024-Badge-Altium-Project-REV1/2024-Badge-BOM-REV1.xlsx
+++ b/Altium/REV1/Project Outputs for 2024-Badge-Altium-Project-REV1/2024-Badge-BOM-REV1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedeaton/plain/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveschw/git/OffensiveSummit/badge-2024/Altium/REV1/Project Outputs for 2024-Badge-Altium-Project-REV1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AB3D51-7519-3E42-AEB4-B03E67AC3C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655007F1-772A-1B41-9031-4A10065A17CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024-Badge-BOM-REV1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="124">
   <si>
     <t>Designator</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>No Solder paste on large GND pad</t>
+  </si>
+  <si>
+    <t>DO NOT PLACE. No Solder paste</t>
+  </si>
+  <si>
+    <t>4 pin-header</t>
   </si>
 </sst>
 </file>
@@ -926,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="207" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1247,8 +1253,8 @@
       <c r="F12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>14</v>
+      <c r="G12" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="H12" s="10">
         <v>41</v>
@@ -1377,8 +1383,8 @@
       <c r="F17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>14</v>
+      <c r="G17" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="H17" s="10">
         <v>1</v>

</xml_diff>